<commit_message>
Added Indian MF 1st Stab
</commit_message>
<xml_diff>
--- a/Reports/MarketBeatRank/2019/T_INV19_BASE/ABBV.xlsx
+++ b/Reports/MarketBeatRank/2019/T_INV19_BASE/ABBV.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7109" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21500" uniqueCount="82">
   <si>
     <t>Mar_10</t>
   </si>
@@ -224,6 +224,48 @@
   </si>
   <si>
     <t>Jun_09</t>
+  </si>
+  <si>
+    <t>Jun_16</t>
+  </si>
+  <si>
+    <t>Jun_24</t>
+  </si>
+  <si>
+    <t>Jun_30</t>
+  </si>
+  <si>
+    <t>6/26/2019,Downgrades,Sell -&gt; Strong Sell,</t>
+  </si>
+  <si>
+    <t>6/26/2019,Reiterates,Hold,</t>
+  </si>
+  <si>
+    <t>Jul_07</t>
+  </si>
+  <si>
+    <t>Jul_17</t>
+  </si>
+  <si>
+    <t>Jul_23</t>
+  </si>
+  <si>
+    <t>Aug_04</t>
+  </si>
+  <si>
+    <t>7/26/2019,Set Price Target,Hold,$80.00</t>
+  </si>
+  <si>
+    <t>Aug_25</t>
+  </si>
+  <si>
+    <t>8/20/2019,Upgrades,Neutral -&gt; Overweight,$80.00</t>
+  </si>
+  <si>
+    <t>Sep_08</t>
+  </si>
+  <si>
+    <t>9/4/2019,Raises Target,Overweight,$80.00 -&gt; $81.00</t>
   </si>
 </sst>
 </file>
@@ -240,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +299,46 @@
         <fgColor indexed="45"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="45"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -270,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="488">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -416,6 +498,294 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="true" borderId="0" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -447,7 +817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -801,84 +1171,120 @@
     <col min="6" max="6" customWidth="true" width="7.1640625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="7.1640625" collapsed="true"/>
     <col min="8" max="8" customWidth="true" width="7.1640625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="31.1640625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="7.1640625" collapsed="true"/>
     <col min="18" max="18" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="31.1640625" collapsed="true"/>
     <col min="20" max="20" customWidth="true" width="8.0" collapsed="true"/>
     <col min="21" max="21" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="8.0" collapsed="false"/>
+    <col min="22" max="22" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="8.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="R1" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="S1" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="T1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="U1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="V1" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="W1" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="X1" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="Y1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Z1" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="AA1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="AB1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="AC1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="AD1" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="AE1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
@@ -949,6 +1355,33 @@
       <c r="V2" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -978,43 +1411,70 @@
       <c r="I3" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>2</v>
-      </c>
       <c r="T3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="U3" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1085,6 +1545,33 @@
       <c r="V4" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1129,28 +1616,55 @@
       <c r="N5" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X5" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="P5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="T5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="U5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="V5" s="0" t="s">
+      <c r="Y5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1219,6 +1733,33 @@
         <v>2</v>
       </c>
       <c r="V6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="0" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1286,7 +1827,34 @@
       <c r="U7" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="V7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1357,6 +1925,33 @@
       <c r="V8" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1410,19 +2005,46 @@
       <c r="Q9" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="S9" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="T9" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="U9" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="V9" s="0" t="s">
+      <c r="AB9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD9" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="0" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1430,14 +2052,14 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>2</v>
+      <c r="B10" s="464" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="432" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="400" t="s">
+        <v>77</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>2</v>
@@ -1491,6 +2113,33 @@
         <v>2</v>
       </c>
       <c r="V10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE10" s="0" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1516,8 +2165,8 @@
       <c r="G11" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>2</v>
+      <c r="H11" s="273" t="s">
+        <v>71</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>2</v>
@@ -1552,13 +2201,40 @@
       <c r="S11" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="T11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="U11" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="V11" s="0" t="s">
+      <c r="AD11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE11" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1629,6 +2305,33 @@
       <c r="V12" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE12" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1694,7 +2397,34 @@
       <c r="U13" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="V13" s="3" t="s">
+      <c r="V13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD13" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE13" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1765,6 +2495,33 @@
       <c r="V14" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE14" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1833,6 +2590,33 @@
       <c r="V15" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD15" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1901,6 +2685,33 @@
       <c r="V16" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE16" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1969,6 +2780,33 @@
       <c r="V17" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -2037,6 +2875,33 @@
       <c r="V18" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD18" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE18" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -2061,7 +2926,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="I19" s="0" t="s">
         <v>2</v>
@@ -2103,6 +2968,33 @@
         <v>2</v>
       </c>
       <c r="V19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD19" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE19" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2171,6 +3063,33 @@
         <v>2</v>
       </c>
       <c r="V20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD20" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE20" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2241,6 +3160,33 @@
       <c r="V21" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE21" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -2309,6 +3255,33 @@
       <c r="V22" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD22" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE22" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -2377,6 +3350,33 @@
       <c r="V23" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD23" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE23" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2445,6 +3445,33 @@
       <c r="V24" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD24" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE24" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -2513,6 +3540,33 @@
       <c r="V25" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE25" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -2581,6 +3635,33 @@
       <c r="V26" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD26" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE26" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -2647,6 +3728,33 @@
         <v>2</v>
       </c>
       <c r="V27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD27" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE27" s="0" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2717,6 +3825,33 @@
       <c r="V28" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="W28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD28" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE28" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -2783,6 +3918,33 @@
         <v>2</v>
       </c>
       <c r="V29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD29" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE29" s="0" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2835,6 +3997,33 @@
       <c r="P30" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="Q30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X30" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y30" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -2885,6 +4074,33 @@
       <c r="P31" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="Q31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="S31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="T31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="V31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="W31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="X31" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y31" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -2908,6 +4124,33 @@
       <c r="G32" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="H32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P32" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
@@ -2929,6 +4172,33 @@
         <v>2</v>
       </c>
       <c r="G33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="M33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="O33" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="P33" s="0" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>